<commit_message>
new test case !!
</commit_message>
<xml_diff>
--- a/src/test/java/com/testbanking/TestData/LoginData.xlsx
+++ b/src/test/java/com/testbanking/TestData/LoginData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12816" windowHeight="4308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16560" windowHeight="4308" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="Addnewcustomer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>mngr83460</t>
   </si>
@@ -44,13 +44,61 @@
   </si>
   <si>
     <t>AjYjAsy</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Birth </t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mobile Number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail </t>
+  </si>
+  <si>
+    <t>anand</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address </t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>fddfd jujddg@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +121,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,8 +143,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,16 +173,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,4 +576,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10101987</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5">
+        <v>678543</v>
+      </c>
+      <c r="H2" s="5">
+        <v>9087654321</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>